<commit_message>
Added Bottom Bar and some Pages
</commit_message>
<xml_diff>
--- a/FoodList.xlsx
+++ b/FoodList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="142">
   <si>
     <t>Products</t>
   </si>
@@ -424,6 +424,30 @@
   </si>
   <si>
     <t>Price on 3/1/2017</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -2039,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,7 +2076,7 @@
     <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2065,8 +2089,11 @@
       <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2079,8 +2106,11 @@
       <c r="D2">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2093,8 +2123,11 @@
       <c r="D3">
         <v>22.57</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2107,8 +2140,11 @@
       <c r="D4">
         <v>31.58</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2121,8 +2157,11 @@
       <c r="D5">
         <v>16.190000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2135,8 +2174,11 @@
       <c r="D6">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2149,8 +2191,11 @@
       <c r="D7">
         <v>12.21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2163,8 +2208,11 @@
       <c r="D8">
         <v>11.86</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2177,8 +2225,11 @@
       <c r="D9">
         <v>7.17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2191,8 +2242,11 @@
       <c r="D10">
         <v>6.69</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2205,8 +2259,11 @@
       <c r="D11">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2219,8 +2276,11 @@
       <c r="D12">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2233,8 +2293,11 @@
       <c r="D13">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2247,8 +2310,11 @@
       <c r="D14">
         <v>2.33</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2261,8 +2327,11 @@
       <c r="D15">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2275,8 +2344,11 @@
       <c r="D16">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2289,8 +2361,11 @@
       <c r="D17">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2303,8 +2378,11 @@
       <c r="D18">
         <v>3.08</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2317,8 +2395,11 @@
       <c r="D19">
         <v>2.81</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2331,8 +2412,11 @@
       <c r="D20">
         <v>3.09</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2345,8 +2429,11 @@
       <c r="D21">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2359,8 +2446,11 @@
       <c r="D22">
         <v>4.91</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2373,8 +2463,11 @@
       <c r="D23">
         <v>4.6100000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2387,8 +2480,11 @@
       <c r="D24">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2401,8 +2497,11 @@
       <c r="D25">
         <v>1.58</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2415,8 +2514,11 @@
       <c r="D26">
         <v>3.74</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2429,8 +2531,11 @@
       <c r="D27">
         <v>3.32</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -2443,8 +2548,11 @@
       <c r="D28">
         <v>2.0699999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -2457,8 +2565,11 @@
       <c r="D29">
         <v>4.1399999999999997</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -2471,8 +2582,11 @@
       <c r="D30">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -2485,8 +2599,11 @@
       <c r="D31">
         <v>2.71</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -2499,8 +2616,11 @@
       <c r="D32">
         <v>8.31</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -2513,8 +2633,11 @@
       <c r="D33">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -2527,8 +2650,11 @@
       <c r="D34">
         <v>6.58</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2541,8 +2667,11 @@
       <c r="D35">
         <v>2.56</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -2555,8 +2684,11 @@
       <c r="D36">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2569,8 +2701,11 @@
       <c r="D37">
         <v>1.54</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -2583,8 +2718,11 @@
       <c r="D38">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -2597,8 +2735,11 @@
       <c r="D39">
         <v>3.21</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -2611,8 +2752,11 @@
       <c r="D40">
         <v>2.83</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -2625,8 +2769,11 @@
       <c r="D41">
         <v>6.44</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -2639,8 +2786,11 @@
       <c r="D42">
         <v>6.85</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -2653,8 +2803,11 @@
       <c r="D43">
         <v>4.53</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -2667,8 +2820,11 @@
       <c r="D44">
         <v>3.99</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2681,8 +2837,11 @@
       <c r="D45">
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -2695,8 +2854,11 @@
       <c r="D46">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -2709,8 +2871,11 @@
       <c r="D47">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -2723,8 +2888,11 @@
       <c r="D48">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -2737,8 +2905,11 @@
       <c r="D49">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -2751,8 +2922,11 @@
       <c r="D50">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -2765,8 +2939,11 @@
       <c r="D51">
         <v>2.69</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -2779,8 +2956,11 @@
       <c r="D52">
         <v>2.68</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -2793,8 +2973,11 @@
       <c r="D53">
         <v>2.54</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -2807,8 +2990,11 @@
       <c r="D54">
         <v>4.05</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -2821,8 +3007,11 @@
       <c r="D55">
         <v>4.6900000000000004</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -2835,24 +3024,42 @@
       <c r="D56">
         <v>2.67</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>132</v>
       </c>
       <c r="B57">
         <v>200</v>
       </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
       <c r="D57">
         <v>103.92</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>89</v>
       </c>
+      <c r="B58" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" t="s">
+        <v>134</v>
+      </c>
       <c r="D58">
         <v>106</v>
+      </c>
+      <c r="E58" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>